<commit_message>
updated rev2.5 hardware outputs
including EMI shield designs and 3D-models
ism + full version BOM listing
</commit_message>
<xml_diff>
--- a/hardware/rev2/assembly/full_bom/cariboulite_r2.5_bom.xlsx
+++ b/hardware/rev2/assembly/full_bom/cariboulite_r2.5_bom.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34551676-2FC9-4F53-B449-541278265884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\cariboulite_hardware\src\manufacturing\rev2\assembly\full_bom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A01B921-7337-4946-ABF4-D1918F441D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{37BEF97A-573F-4D07-8F82-9F2C2AE77A39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EC062A6-726F-49B1-B1BB-44F17A238F12}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-CaribouLite(Caribo" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="211">
   <si>
     <t>Designator</t>
   </si>
@@ -256,7 +261,7 @@
     <t>D3, D4</t>
   </si>
   <si>
-    <t>LXES15AAA1-153</t>
+    <t>0402ESDB-MLP1</t>
   </si>
   <si>
     <t>ESD Suppressors / TVS Diodes ESD Protection Device, 0402, Bidirectional, 4V working, 15V breakdown, 0.05pF Cd</t>
@@ -302,6 +307,18 @@
   </si>
   <si>
     <t>10129383912001ALF</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>CONUFL001-SMD-T</t>
+  </si>
+  <si>
+    <t>RF Connectors / Coaxial Connectors U.FL Straight Surface Mount Jack</t>
+  </si>
+  <si>
+    <t>LINX_CONUFL001-SMD-T</t>
   </si>
   <si>
     <t>L1, L2, L4, L5, L13, L14, L15, L18, L20, L21</t>
@@ -712,13 +729,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,20 +1052,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9595163-FB2C-461C-8A30-851BAEF8440D}">
-  <dimension ref="A1:G50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB401062-8B70-4F02-8EE0-4B0952458D22}">
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1072,7 +1094,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1095,7 +1117,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1117,8 +1139,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1141,7 +1163,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1164,7 +1186,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1186,8 +1208,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1209,8 +1231,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1233,7 +1255,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1256,7 +1278,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1279,7 +1301,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1302,7 +1324,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1325,7 +1347,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1348,7 +1370,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1371,7 +1393,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1394,7 +1416,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1417,7 +1439,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1440,7 +1462,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1463,7 +1485,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1486,7 +1508,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1509,7 +1531,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1532,14 +1554,14 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>71</v>
@@ -1555,83 +1577,83 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C23" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="3">
+      <c r="E24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="3">
         <v>11</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="3">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>111</v>
@@ -1640,14 +1662,14 @@
         <v>112</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1663,21 +1685,21 @@
         <v>116</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C28" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>119</v>
@@ -1686,21 +1708,21 @@
         <v>120</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>123</v>
@@ -1709,21 +1731,21 @@
         <v>124</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C30" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>127</v>
@@ -1732,41 +1754,41 @@
         <v>128</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C31" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>132</v>
+      <c r="A32" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -1775,17 +1797,17 @@
         <v>71</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1808,7 +1830,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1818,47 +1840,47 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>148</v>
+      <c r="A36" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -1867,17 +1889,17 @@
         <v>71</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1900,14 +1922,14 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>71</v>
@@ -1923,14 +1945,14 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>71</v>
@@ -1946,14 +1968,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>71</v>
@@ -1969,14 +1991,14 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>71</v>
@@ -1985,44 +2007,44 @@
         <v>170</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>171</v>
+      <c r="A42" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C42" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>71</v>
@@ -2038,14 +2060,14 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="4" t="s">
         <v>179</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>71</v>
@@ -2054,37 +2076,37 @@
         <v>181</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>182</v>
+      <c r="A45" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2107,7 +2129,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2130,7 +2152,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="4" t="s">
         <v>194</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2149,41 +2171,41 @@
         <v>197</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="3">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C49" s="3">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C50" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>71</v>
@@ -2198,8 +2220,31 @@
         <v>204</v>
       </c>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>